<commit_message>
Updated spreadsheet for 2016 labs
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2016.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2016.xlsx
@@ -2157,11 +2157,11 @@
   <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7632" ySplit="864" topLeftCell="D1" activePane="bottomRight"/>
+      <pane xSplit="7632" ySplit="864" topLeftCell="I1" activePane="bottomRight"/>
       <selection activeCell="B46" sqref="B46"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2325,11 +2325,11 @@
         <v>0</v>
       </c>
       <c r="P3" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O3,D$2:D$76)</f>
+        <f t="shared" ref="P3:P11" si="3">SUMIF(N$2:N$76,"&gt;=" &amp; O3,D$2:D$76)</f>
         <v>289</v>
       </c>
       <c r="Q3" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O3,E$2:E$76)</f>
+        <f t="shared" ref="Q3:Q11" si="4">SUMIF(N$2:N$76,"&gt;=" &amp; O3,E$2:E$76)</f>
         <v>19</v>
       </c>
       <c r="R3" s="11">
@@ -2342,7 +2342,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="17" t="str">
-        <f t="shared" ref="C4:C24" si="3">RIGHT(B4,2)</f>
+        <f t="shared" ref="C4:C24" si="5">RIGHT(B4,2)</f>
         <v>15</v>
       </c>
       <c r="D4" s="19">
@@ -2373,16 +2373,16 @@
         <v>0.5</v>
       </c>
       <c r="P4" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O4,D$2:D$76)</f>
-        <v>206</v>
+        <f t="shared" si="3"/>
+        <v>204</v>
       </c>
       <c r="Q4" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O4,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="R4" s="11">
-        <f t="shared" ref="R4:R11" si="4">$Q$16 + $Q$14*P4+($Q$15-$Q$14)*Q4</f>
-        <v>16.600000000000001</v>
+        <f t="shared" ref="R4:R11" si="6">$Q$16 + $Q$14*P4+($Q$15-$Q$14)*Q4</f>
+        <v>16.5</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="D5" s="18">
@@ -2432,16 +2432,16 @@
         <v>1</v>
       </c>
       <c r="P5" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O5,D$2:D$76)</f>
-        <v>201</v>
+        <f t="shared" si="3"/>
+        <v>199</v>
       </c>
       <c r="Q5" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O5,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="R5" s="11">
-        <f t="shared" si="4"/>
-        <v>16.350000000000001</v>
+        <f t="shared" si="6"/>
+        <v>16.25</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -2449,7 +2449,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="D6" s="19">
@@ -2475,15 +2475,15 @@
         <v>1.5</v>
       </c>
       <c r="P6" s="48">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O6,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="Q6" s="48">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O6,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="R6" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.700000000000001</v>
       </c>
     </row>
@@ -2492,7 +2492,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="D7" s="19">
@@ -2527,15 +2527,15 @@
         <v>2</v>
       </c>
       <c r="P7" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O7,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="Q7" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O7,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="R7" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.700000000000001</v>
       </c>
     </row>
@@ -2544,7 +2544,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="D8" s="19">
@@ -2573,15 +2573,15 @@
         <v>2.5</v>
       </c>
       <c r="P8" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O8,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="Q8" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O8,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R8" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.6</v>
       </c>
     </row>
@@ -2590,7 +2590,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="D9" s="19">
@@ -2631,15 +2631,15 @@
         <v>3</v>
       </c>
       <c r="P9" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O9,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="Q9" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O9,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="R9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.6000000000000014</v>
       </c>
     </row>
@@ -2648,7 +2648,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="D10" s="19">
@@ -2685,15 +2685,15 @@
         <v>3.5</v>
       </c>
       <c r="P10" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O10,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="Q10" s="8">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O10,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R10" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.9</v>
       </c>
     </row>
@@ -2702,7 +2702,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="D11" s="19">
@@ -2736,15 +2736,15 @@
         <v>4</v>
       </c>
       <c r="P11" s="23">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O11,D$2:D$76)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="Q11" s="23">
-        <f>SUMIF(N$2:N$76,"&gt;=" &amp; O11,E$2:E$76)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R11" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.15</v>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="D12" s="19">
@@ -2792,7 +2792,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="D13" s="19">
@@ -2834,7 +2834,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="D14" s="19">
@@ -2877,7 +2877,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="D15" s="19">
@@ -2920,7 +2920,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="D16" s="19">
@@ -2963,7 +2963,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="D17" s="19">
@@ -3000,7 +3000,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="D18" s="19">
@@ -3031,7 +3031,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
       <c r="D19" s="19">
@@ -3065,7 +3065,7 @@
         <v>30</v>
       </c>
       <c r="C20" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
       <c r="D20" s="19">
@@ -3102,7 +3102,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="D21" s="18">
@@ -3144,7 +3144,7 @@
         <v>32</v>
       </c>
       <c r="C22" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
       <c r="D22" s="19">
@@ -3186,7 +3186,7 @@
         <v>33</v>
       </c>
       <c r="C23" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>93</v>
       </c>
       <c r="D23" s="19">
@@ -3220,7 +3220,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="D24" s="19">
@@ -3292,7 +3292,7 @@
         <v>35</v>
       </c>
       <c r="C26" s="17" t="str">
-        <f t="shared" ref="C26:C75" si="5">RIGHT(B26,3)</f>
+        <f t="shared" ref="C26:C75" si="7">RIGHT(B26,3)</f>
         <v>104</v>
       </c>
       <c r="D26" s="19">
@@ -3334,7 +3334,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>107</v>
       </c>
       <c r="D27" s="19">
@@ -3364,7 +3364,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>110</v>
       </c>
       <c r="D28" s="19">
@@ -3395,7 +3395,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>115</v>
       </c>
       <c r="D29" s="19">
@@ -3426,7 +3426,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="D30" s="18">
@@ -3462,7 +3462,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>123</v>
       </c>
       <c r="D31" s="19">
@@ -3499,7 +3499,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>126</v>
       </c>
       <c r="D32" s="19">
@@ -3542,7 +3542,7 @@
         <v>42</v>
       </c>
       <c r="C33" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>129</v>
       </c>
       <c r="D33" s="19">
@@ -3576,7 +3576,7 @@
         <v>143</v>
       </c>
       <c r="C34" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Law</v>
       </c>
       <c r="D34" s="19">
@@ -3611,7 +3611,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>132</v>
       </c>
       <c r="D35" s="19">
@@ -3645,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="N35" s="40">
-        <f t="shared" ref="N35:N66" si="6">SUM(I35:L35)</f>
+        <f t="shared" ref="N35:N66" si="8">SUM(I35:L35)</f>
         <v>4</v>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
         <v>44</v>
       </c>
       <c r="C36" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>139</v>
       </c>
       <c r="D36" s="18">
@@ -3691,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.7</v>
       </c>
       <c r="O36" s="20"/>
@@ -3701,7 +3701,7 @@
         <v>45</v>
       </c>
       <c r="C37" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>141</v>
       </c>
       <c r="D37" s="19">
@@ -3735,7 +3735,7 @@
         <v>1</v>
       </c>
       <c r="N37" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.7</v>
       </c>
     </row>
@@ -3744,7 +3744,7 @@
         <v>46</v>
       </c>
       <c r="C38" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>146</v>
       </c>
       <c r="D38" s="19">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="H38" s="36"/>
       <c r="N38" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
         <v>47</v>
       </c>
       <c r="C39" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="D39" s="19">
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="N39" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3808,7 +3808,7 @@
         <v>48</v>
       </c>
       <c r="C40" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156</v>
       </c>
       <c r="D40" s="19">
@@ -3840,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="N40" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="N41" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="O41" s="20"/>
@@ -3926,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="N42" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.5</v>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
         <v>85</v>
       </c>
       <c r="C43" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>171</v>
       </c>
       <c r="D43" s="19">
@@ -3955,15 +3955,12 @@
       <c r="H43" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="J43" s="3">
-        <v>1</v>
-      </c>
       <c r="M43" s="3">
         <v>1</v>
       </c>
       <c r="N43" s="40">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -3971,7 +3968,7 @@
         <v>86</v>
       </c>
       <c r="C44" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>173</v>
       </c>
       <c r="D44" s="19">
@@ -4002,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="N44" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -4014,7 +4011,7 @@
         <v>103</v>
       </c>
       <c r="C45" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>175</v>
       </c>
       <c r="D45" s="18">
@@ -4042,7 +4039,7 @@
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="O45" s="20"/>
@@ -4052,7 +4049,7 @@
         <v>104</v>
       </c>
       <c r="C46" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>178</v>
       </c>
       <c r="D46" s="19">
@@ -4077,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -4089,7 +4086,7 @@
         <v>105</v>
       </c>
       <c r="C47" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>180</v>
       </c>
       <c r="D47" s="18">
@@ -4117,7 +4114,7 @@
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="O47" s="20"/>
@@ -4127,7 +4124,7 @@
         <v>134</v>
       </c>
       <c r="C48" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>182</v>
       </c>
       <c r="D48" s="19">
@@ -4152,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="N48" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -4161,7 +4158,7 @@
         <v>131</v>
       </c>
       <c r="C49" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>186</v>
       </c>
       <c r="D49" s="19">
@@ -4183,7 +4180,7 @@
         <v>1</v>
       </c>
       <c r="N49" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4192,7 +4189,7 @@
         <v>106</v>
       </c>
       <c r="C50" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>189</v>
       </c>
       <c r="D50" s="19">
@@ -4214,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="N50" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4223,7 +4220,7 @@
         <v>107</v>
       </c>
       <c r="C51" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="D51" s="19">
@@ -4245,7 +4242,7 @@
         <v>1</v>
       </c>
       <c r="N51" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4254,7 +4251,7 @@
         <v>108</v>
       </c>
       <c r="C52" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="D52" s="19">
@@ -4282,7 +4279,7 @@
         <v>1</v>
       </c>
       <c r="N52" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -4291,7 +4288,7 @@
         <v>109</v>
       </c>
       <c r="C53" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>199</v>
       </c>
       <c r="D53" s="19">
@@ -4316,7 +4313,7 @@
         <v>1</v>
       </c>
       <c r="N53" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2</v>
       </c>
     </row>
@@ -4325,7 +4322,7 @@
         <v>110</v>
       </c>
       <c r="C54" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>204</v>
       </c>
       <c r="D54" s="19">
@@ -4355,7 +4352,7 @@
         <v>1</v>
       </c>
       <c r="N54" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -4364,7 +4361,7 @@
         <v>132</v>
       </c>
       <c r="C55" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>205</v>
       </c>
       <c r="D55" s="19">
@@ -4385,7 +4382,7 @@
         <v>7</v>
       </c>
       <c r="N55" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4394,7 +4391,7 @@
         <v>111</v>
       </c>
       <c r="C56" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>207</v>
       </c>
       <c r="D56" s="19">
@@ -4418,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="N56" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -4427,7 +4424,7 @@
         <v>112</v>
       </c>
       <c r="C57" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212</v>
       </c>
       <c r="D57" s="19">
@@ -4449,7 +4446,7 @@
         <v>1</v>
       </c>
       <c r="N57" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4458,7 +4455,7 @@
         <v>113</v>
       </c>
       <c r="C58" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>221</v>
       </c>
       <c r="D58" s="19">
@@ -4480,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="N58" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4492,7 +4489,7 @@
         <v>114</v>
       </c>
       <c r="C59" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>228</v>
       </c>
       <c r="D59" s="18">
@@ -4520,7 +4517,7 @@
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="O59" s="20"/>
@@ -4530,7 +4527,7 @@
         <v>115</v>
       </c>
       <c r="C60" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>231</v>
       </c>
       <c r="D60" s="19">
@@ -4549,7 +4546,7 @@
       </c>
       <c r="H60" s="36"/>
       <c r="N60" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4558,7 +4555,7 @@
         <v>116</v>
       </c>
       <c r="C61" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>238</v>
       </c>
       <c r="D61" s="19">
@@ -4577,7 +4574,7 @@
       </c>
       <c r="H61" s="36"/>
       <c r="N61" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4586,7 +4583,7 @@
         <v>117</v>
       </c>
       <c r="C62" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>245</v>
       </c>
       <c r="D62" s="19">
@@ -4608,7 +4605,7 @@
         <v>1</v>
       </c>
       <c r="N62" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -4620,7 +4617,7 @@
         <v>118</v>
       </c>
       <c r="C63" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>255</v>
       </c>
       <c r="D63" s="18">
@@ -4644,7 +4641,7 @@
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
       <c r="N63" s="39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O63" s="20"/>
@@ -4654,7 +4651,7 @@
         <v>119</v>
       </c>
       <c r="C64" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>261</v>
       </c>
       <c r="D64" s="19">
@@ -4673,7 +4670,7 @@
       </c>
       <c r="H64" s="36"/>
       <c r="N64" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4682,7 +4679,7 @@
         <v>120</v>
       </c>
       <c r="C65" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>264</v>
       </c>
       <c r="D65" s="19">
@@ -4701,7 +4698,7 @@
       </c>
       <c r="H65" s="36"/>
       <c r="N65" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4710,7 +4707,7 @@
         <v>121</v>
       </c>
       <c r="C66" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>268</v>
       </c>
       <c r="D66" s="19">
@@ -4729,7 +4726,7 @@
       </c>
       <c r="H66" s="36"/>
       <c r="N66" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4738,7 +4735,7 @@
         <v>122</v>
       </c>
       <c r="C67" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>272</v>
       </c>
       <c r="D67" s="19">
@@ -4757,7 +4754,7 @@
       </c>
       <c r="H67" s="36"/>
       <c r="N67" s="40">
-        <f t="shared" ref="N67:N75" si="7">SUM(I67:L67)</f>
+        <f t="shared" ref="N67:N75" si="9">SUM(I67:L67)</f>
         <v>0</v>
       </c>
     </row>
@@ -4769,7 +4766,7 @@
         <v>123</v>
       </c>
       <c r="C68" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>275</v>
       </c>
       <c r="D68" s="18">
@@ -4780,7 +4777,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="25">
-        <f t="shared" ref="F68:F75" si="8">$Q$14*D68+($Q$15-$Q$14)*E68</f>
+        <f t="shared" ref="F68:F75" si="10">$Q$14*D68+($Q$15-$Q$14)*E68</f>
         <v>0.1</v>
       </c>
       <c r="G68" s="15"/>
@@ -4799,7 +4796,7 @@
       </c>
       <c r="M68" s="15"/>
       <c r="N68" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O68" s="20"/>
@@ -4809,18 +4806,18 @@
         <v>124</v>
       </c>
       <c r="C69" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>277</v>
       </c>
       <c r="D69" s="19">
-        <f t="shared" ref="D69:D74" si="9">C70-C69</f>
+        <f t="shared" ref="D69:D74" si="11">C70-C69</f>
         <v>2</v>
       </c>
       <c r="E69" s="19">
         <v>1</v>
       </c>
       <c r="F69" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.4</v>
       </c>
       <c r="H69" s="36"/>
@@ -4837,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="N69" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -4846,18 +4843,18 @@
         <v>125</v>
       </c>
       <c r="C70" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>279</v>
       </c>
       <c r="D70" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="E70" s="19">
         <v>3</v>
       </c>
       <c r="F70" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="H70" s="36"/>
@@ -4874,7 +4871,7 @@
         <v>1</v>
       </c>
       <c r="N70" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -4883,18 +4880,18 @@
         <v>126</v>
       </c>
       <c r="C71" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>283</v>
       </c>
       <c r="D71" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E71" s="19">
         <v>0</v>
       </c>
       <c r="F71" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.05</v>
       </c>
       <c r="H71" s="36" t="s">
@@ -4910,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="N71" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -4919,25 +4916,25 @@
         <v>127</v>
       </c>
       <c r="C72" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>284</v>
       </c>
       <c r="D72" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E72" s="19">
         <v>0</v>
       </c>
       <c r="F72" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.1</v>
       </c>
       <c r="H72" s="36" t="s">
         <v>7</v>
       </c>
       <c r="N72" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4946,23 +4943,23 @@
         <v>128</v>
       </c>
       <c r="C73" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>286</v>
       </c>
       <c r="D73" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E73" s="19">
         <v>1</v>
       </c>
       <c r="F73" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.45</v>
       </c>
       <c r="H73" s="36"/>
       <c r="N73" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4971,23 +4968,23 @@
         <v>129</v>
       </c>
       <c r="C74" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>289</v>
       </c>
       <c r="D74" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E74" s="19">
         <v>0</v>
       </c>
       <c r="F74" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.05</v>
       </c>
       <c r="H74" s="36"/>
       <c r="N74" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4996,7 +4993,7 @@
         <v>130</v>
       </c>
       <c r="C75" s="52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>290</v>
       </c>
       <c r="D75" s="53">
@@ -5006,7 +5003,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.2</v>
       </c>
       <c r="G75" s="54"/>
@@ -5017,7 +5014,7 @@
       <c r="L75" s="54"/>
       <c r="M75" s="54"/>
       <c r="N75" s="56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5119,7 +5116,7 @@
       </c>
       <c r="J81" s="33">
         <f t="array" ref="J81">SUM($D2:$D75*J2:J75*($N2:$N75&lt;$P$19))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K81" s="33">
         <f t="array" ref="K81">SUM($D2:$D75*K2:K75*($N2:$N75&lt;$P$19))</f>

</xml_diff>

<commit_message>
Jack decided to do another lab this spring
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2016.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2016.xlsx
@@ -2160,8 +2160,8 @@
       <pane xSplit="7632" ySplit="864" topLeftCell="I1" activePane="bottomRight"/>
       <selection activeCell="B46" sqref="B46"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="P6" s="48">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q6" s="48">
         <f t="shared" si="4"/>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="R6" s="49">
         <f t="shared" si="6"/>
-        <v>12.700000000000001</v>
+        <v>12.950000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="P7" s="8">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="4"/>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="R7" s="11">
         <f t="shared" si="6"/>
-        <v>12.700000000000001</v>
+        <v>12.950000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -2562,12 +2562,15 @@
         <v>15</v>
       </c>
       <c r="H8" s="36"/>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
       <c r="K8" s="3">
         <v>1</v>
       </c>
       <c r="N8" s="40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="20">
         <v>2.5</v>
@@ -5028,11 +5031,11 @@
       </c>
       <c r="J77" s="15">
         <f t="array" ref="J77">SUM($D2:$D75*(J2:J75&gt;=0.9)*($N2:$N75&gt;=$P$19))</f>
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="K77" s="15">
         <f t="array" ref="K77">SUM($D2:$D75*(K2:K75&gt;=0.9)*($N2:$N75&gt;=$P$19))</f>
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L77" s="35">
         <f t="array" ref="L77">SUM($D2:$D75*(L2:L75&gt;=0.9)*($N2:$N75&gt;=$P$19))</f>
@@ -5050,11 +5053,11 @@
       </c>
       <c r="J78" s="33">
         <f t="array" ref="J78">SUM($D2:$D75*J2:J75*($N2:$N75&gt;=$P$19))</f>
-        <v>98.5</v>
+        <v>103.5</v>
       </c>
       <c r="K78" s="33">
         <f t="array" ref="K78">SUM($D2:$D75*K2:K75*($N2:$N75&gt;=$P$19))</f>
-        <v>109.4</v>
+        <v>114.4</v>
       </c>
       <c r="L78" s="36">
         <f t="array" ref="L78">SUM($D2:$D75*L2:L75*($N2:$N75&gt;=$P$19))</f>
@@ -5068,19 +5071,19 @@
       </c>
       <c r="I79" s="58">
         <f>I78/$P$6</f>
-        <v>0.80136986301369861</v>
+        <v>0.77483443708609268</v>
       </c>
       <c r="J79" s="58">
         <f>J78/$P$6</f>
-        <v>0.67465753424657537</v>
+        <v>0.68543046357615889</v>
       </c>
       <c r="K79" s="58">
         <f>K78/$P$6</f>
-        <v>0.74931506849315077</v>
+        <v>0.75761589403973517</v>
       </c>
       <c r="L79" s="59">
         <f>L78/$P$6</f>
-        <v>0.77397260273972601</v>
+        <v>0.7483443708609272</v>
       </c>
       <c r="M79" s="36"/>
     </row>
@@ -5094,11 +5097,11 @@
       </c>
       <c r="J80" s="33">
         <f t="array" ref="J80">SUM($D2:$D75*(J2:J75&gt;=0.1)*($N2:$N75&gt;=$P$19))</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="K80" s="33">
         <f t="array" ref="K80">SUM($D2:$D75*(K2:K75&gt;=0.1)*($N2:$N75&gt;=$P$19))</f>
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="L80" s="36">
         <f t="array" ref="L80">SUM($D2:$D75*(L2:L75&gt;=0.1)*($N2:$N75&gt;=$P$19))</f>
@@ -5120,7 +5123,7 @@
       </c>
       <c r="K81" s="33">
         <f t="array" ref="K81">SUM($D2:$D75*K2:K75*($N2:$N75&lt;$P$19))</f>
-        <v>21.5</v>
+        <v>16.5</v>
       </c>
       <c r="L81" s="36">
         <f t="array" ref="L81">SUM($D2:$D75*L2:L75*($N2:$N75&lt;$P$19))</f>

</xml_diff>